<commit_message>
Added Big tech models overview file and AAPL model
</commit_message>
<xml_diff>
--- a/Big Tech/Accenture.xlsx
+++ b/Big Tech/Accenture.xlsx
@@ -5,24 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/To Be Modeled/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Big Tech/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFF4DAA-3416-824A-A3B9-62A70D4CB611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00BEA6D-5F21-D94B-B474-7E39CF484C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Sheet 1'!$A$106</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Sheet 1'!$A$19</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Sheet 1'!$A$3</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Sheet 1'!$B$106:$W$106</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Sheet 1'!$B$19:$W$19</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Sheet 1'!$B$3:$W$3</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,8 +32,45 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="160">
   <si>
     <t>INCOME STATEMENT (in mln.)</t>
   </si>
@@ -323,9 +352,6 @@
   </si>
   <si>
     <t>link</t>
-  </si>
-  <si>
-    <t>Accenture</t>
   </si>
   <si>
     <t>Revenue Growth YoY</t>
@@ -866,7 +892,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -930,18 +956,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -951,12 +965,7 @@
     </xf>
     <xf numFmtId="10" fontId="12" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="11" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="11" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="16" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -978,12 +987,6 @@
     <xf numFmtId="10" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -995,10 +998,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="12" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1006,6 +1005,27 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="11" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2235,6 +2255,446 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+  <types>
+    <type name="_linkedentity">
+      <keyFlags>
+        <key name="%cvi">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+      </keyFlags>
+    </type>
+    <type name="_linkedentitycore">
+      <keyFlags>
+        <key name="%EntityServiceId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntitySubDomainId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntityCulture">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntityId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%IsRefreshable">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+        <key name="%ProviderInfo">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%DataProviderExternalLinkLogo">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%DataProviderExternalLink">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%OutdatedReason">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+      </keyFlags>
+    </type>
+  </types>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1mthw&amp;q=XNYS%3aACN&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>ACCENTURE PUBLIC LIMITED COMPANY (XNYS:ACN)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-US</v>
+    <v>a1mthw</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>345.29500000000002</v>
+    <v>242.8</v>
+    <v>1.2434000000000001</v>
+    <v>3.15</v>
+    <v>1.1144000000000001E-2</v>
+    <v>0.19</v>
+    <v>6.648E-4</v>
+    <v>USD</v>
+    <v>Accenture plc is a global professional services company engaged in providing a range of services in strategy and consulting, technology, operations and Accenture song. It serves clients in North America, Europe and Growth markets. It provides a range of services, including application services, artificial intelligence, automation, business process outsourcing, business strategy, change management, cloud, data and analytics, digital commerce, digital engineering and manufacturing, finance consulting, infrastructure, marketing, mergers and acquisitions, metaverse, operating models, security, supply chain management, technology consulting, technology innovation and zero-based transformation. It helps organizations to achieve transformational impact with solutions in C-Suite assessment, team dynamics and various others. It also offers automated production lines that leverage the cloud, data and artificial intelligence (AI) that makes factories and plants smarter through Eclipse Automation.</v>
+    <v>721000</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>1 Grand Canal Square, Grand Canal Harbour, Dublin 2, DUBLIN, DUBLIN IE</v>
+    <v>285.95999999999998</v>
+    <v>Software &amp; IT Services</v>
+    <v>Stock</v>
+    <v>45016.992773471873</v>
+    <v>0</v>
+    <v>282.61</v>
+    <v>189376500000</v>
+    <v>ACCENTURE PUBLIC LIMITED COMPANY</v>
+    <v>ACCENTURE PUBLIC LIMITED COMPANY</v>
+    <v>283.12</v>
+    <v>26.017099999999999</v>
+    <v>282.66000000000003</v>
+    <v>285.81</v>
+    <v>286</v>
+    <v>662595700</v>
+    <v>ACN</v>
+    <v>ACCENTURE PUBLIC LIMITED COMPANY (XNYS:ACN)</v>
+    <v>3009370</v>
+    <v>2885890</v>
+    <v>2009</v>
+  </rv>
+  <rv s="2">
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
+  <s t="_hyperlink">
+    <k n="Address" t="s"/>
+    <k n="Text" t="s"/>
+  </s>
+  <s t="_linkedentitycore">
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="%ProviderInfo" t="s"/>
+    <k n="52 week high"/>
+    <k n="52 week low"/>
+    <k n="Beta"/>
+    <k n="Change"/>
+    <k n="Change (%)"/>
+    <k n="Change (Extended hours)"/>
+    <k n="Change % (Extended hours)"/>
+    <k n="Currency" t="s"/>
+    <k n="Description" t="s"/>
+    <k n="Employees"/>
+    <k n="Exchange" t="s"/>
+    <k n="Exchange abbreviation" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Headquarters" t="s"/>
+    <k n="High"/>
+    <k n="Industry" t="s"/>
+    <k n="Instrument type" t="s"/>
+    <k n="Last trade time"/>
+    <k n="LearnMoreOnLink" t="r"/>
+    <k n="Low"/>
+    <k n="Market cap"/>
+    <k n="Name" t="s"/>
+    <k n="Official name" t="s"/>
+    <k n="Open"/>
+    <k n="P/E"/>
+    <k n="Previous close"/>
+    <k n="Price"/>
+    <k n="Price (Extended hours)"/>
+    <k n="Shares outstanding"/>
+    <k n="Ticker symbol" t="s"/>
+    <k n="UniqueName" t="s"/>
+    <k n="Volume"/>
+    <k n="Volume average"/>
+    <k n="Year incorporated"/>
+  </s>
+  <s t="_linkedentity">
+    <k n="%cvi" t="r"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
+<supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <spbArrays count="1">
+    <a count="45">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">_Format</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">_Display</v>
+      <v t="s">Name</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Price</v>
+      <v t="s">Price (Extended hours)</v>
+      <v t="s">Exchange</v>
+      <v t="s">Official name</v>
+      <v t="s">Last trade time</v>
+      <v t="s">Ticker symbol</v>
+      <v t="s">Exchange abbreviation</v>
+      <v t="s">Change</v>
+      <v t="s">Change (Extended hours)</v>
+      <v t="s">Change (%)</v>
+      <v t="s">Change % (Extended hours)</v>
+      <v t="s">Currency</v>
+      <v t="s">Previous close</v>
+      <v t="s">Open</v>
+      <v t="s">High</v>
+      <v t="s">Low</v>
+      <v t="s">52 week high</v>
+      <v t="s">52 week low</v>
+      <v t="s">Volume</v>
+      <v t="s">Volume average</v>
+      <v t="s">Market cap</v>
+      <v t="s">Beta</v>
+      <v t="s">P/E</v>
+      <v t="s">Shares outstanding</v>
+      <v t="s">Description</v>
+      <v t="s">Employees</v>
+      <v t="s">Headquarters</v>
+      <v t="s">Industry</v>
+      <v t="s">Instrument type</v>
+      <v t="s">Year incorporated</v>
+      <v t="s">_Flags</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">LearnMoreOnLink</v>
+      <v t="s">ExchangeID</v>
+      <v t="s">%ProviderInfo</v>
+    </a>
+  </spbArrays>
+  <spbData count="5">
+    <spb s="0">
+      <v>0</v>
+      <v>Name</v>
+      <v>LearnMoreOnLink</v>
+    </spb>
+    <spb s="1">
+      <v>0</v>
+      <v>0</v>
+      <v>0</v>
+    </spb>
+    <spb s="2">
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+    </spb>
+    <spb s="3">
+      <v>1</v>
+      <v>2</v>
+      <v>2</v>
+      <v>1</v>
+      <v>3</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>4</v>
+      <v>5</v>
+      <v>6</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>7</v>
+      <v>8</v>
+      <v>9</v>
+      <v>4</v>
+      <v>1</v>
+      <v>1</v>
+      <v>5</v>
+    </spb>
+    <spb s="4">
+      <v>at close</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq</v>
+      <v>GMT</v>
+      <v>Delayed 15 minutes</v>
+      <v>from close</v>
+      <v>from close</v>
+    </spb>
+  </spbData>
+</supportingPropertyBags>
+</file>
+
+<file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="5">
+  <s>
+    <k n="^Order" t="spba"/>
+    <k n="TitleProperty" t="s"/>
+    <k n="SubTitleProperty" t="s"/>
+  </s>
+  <s>
+    <k n="ShowInCardView" t="b"/>
+    <k n="ShowInDotNotation" t="b"/>
+    <k n="ShowInAutoComplete" t="b"/>
+  </s>
+  <s>
+    <k n="ExchangeID" t="spb"/>
+    <k n="UniqueName" t="spb"/>
+    <k n="`%ProviderInfo" t="spb"/>
+    <k n="LearnMoreOnLink" t="spb"/>
+  </s>
+  <s>
+    <k n="Low" t="i"/>
+    <k n="P/E" t="i"/>
+    <k n="Beta" t="i"/>
+    <k n="High" t="i"/>
+    <k n="Name" t="i"/>
+    <k n="Open" t="i"/>
+    <k n="Price" t="i"/>
+    <k n="Change" t="i"/>
+    <k n="Volume" t="i"/>
+    <k n="Employees" t="i"/>
+    <k n="Change (%)" t="i"/>
+    <k n="Market cap" t="i"/>
+    <k n="52 week low" t="i"/>
+    <k n="52 week high" t="i"/>
+    <k n="Previous close" t="i"/>
+    <k n="Volume average" t="i"/>
+    <k n="Last trade time" t="i"/>
+    <k n="Year incorporated" t="i"/>
+    <k n="`%EntityServiceId" t="i"/>
+    <k n="Shares outstanding" t="i"/>
+    <k n="Price (Extended hours)" t="i"/>
+    <k n="Change (Extended hours)" t="i"/>
+    <k n="Change % (Extended hours)" t="i"/>
+  </s>
+  <s>
+    <k n="Price" t="s"/>
+    <k n="Change" t="s"/>
+    <k n="Change (%)" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Last trade time" t="s"/>
+    <k n="Price (Extended hours)" t="s"/>
+    <k n="Change (Extended hours)" t="s"/>
+    <k n="Change % (Extended hours)" t="s"/>
+  </s>
+</spbStructures>
+</file>
+
+<file path=xl/richData/richStyles.xml><?xml version="1.0" encoding="utf-8"?>
+<richStyleSheet xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <dxfs count="7">
+    <x:dxf>
+      <x:numFmt numFmtId="2" formatCode="0.00"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="0" formatCode="General"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="27" formatCode="m/d/yy\ h:mm"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="14" formatCode="0.00%"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="3" formatCode="#,##0"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="1" formatCode="0"/>
+    </x:dxf>
+  </dxfs>
+  <richProperties>
+    <rPr n="NumberFormat" t="s"/>
+    <rPr n="IsTitleField" t="b"/>
+  </richProperties>
+  <richStyles>
+    <rSty dxfid="1">
+      <rpv i="0">_([$$-en-US]* #,##0.00_);_([$$-en-US]* (#,##0.00);_([$$-en-US]* "-"??_);_(@_)</rpv>
+    </rSty>
+    <rSty dxfid="5">
+      <rpv i="0">#,##0.00</rpv>
+    </rSty>
+    <rSty>
+      <rpv i="1">1</rpv>
+    </rSty>
+    <rSty dxfid="4">
+      <rpv i="0">#,##0</rpv>
+    </rSty>
+    <rSty dxfid="3"/>
+    <rSty dxfid="1">
+      <rpv i="0">_([$$-en-US]* #,##0_);_([$$-en-US]* (#,##0);_([$$-en-US]* "-"_);_(@_)</rpv>
+    </rSty>
+    <rSty dxfid="2"/>
+    <rSty dxfid="6">
+      <rpv i="0">0</rpv>
+    </rSty>
+    <rSty dxfid="0">
+      <rpv i="0">0.00</rpv>
+    </rSty>
+  </richStyles>
+</richStyleSheet>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2535,10 +2995,10 @@
   <dimension ref="A1:AF118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="W103" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AH117" sqref="AH117"/>
+      <selection pane="bottomRight" activeCell="Y124" sqref="Y124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2549,8 +3009,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>94</v>
+      <c r="A1" s="3" t="e" vm="1">
+        <v>#VALUE!</v>
       </c>
       <c r="B1" s="8">
         <v>2001</v>
@@ -2806,21 +3266,21 @@
         <v>82216000000</v>
       </c>
       <c r="AC3" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD3" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="AD3" s="19" t="s">
+      <c r="AE3" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="AE3" s="19" t="s">
+      <c r="AF3" s="19" t="s">
         <v>112</v>
-      </c>
-      <c r="AF3" s="19" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="15">
@@ -3086,16 +3546,16 @@
         <v>19701539000</v>
       </c>
       <c r="AC6" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD6" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="AD6" s="19" t="s">
+      <c r="AE6" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="AE6" s="19" t="s">
+      <c r="AF6" s="19" t="s">
         <v>116</v>
-      </c>
-      <c r="AF6" s="19" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="19" x14ac:dyDescent="0.25">
@@ -3258,7 +3718,7 @@
     </row>
     <row r="9" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="15">
         <f>B8/B3</f>
@@ -3349,16 +3809,16 @@
         <v>0</v>
       </c>
       <c r="AC9" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD9" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="AD9" s="19" t="s">
+      <c r="AE9" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="AE9" s="19" t="s">
+      <c r="AF9" s="19" t="s">
         <v>99</v>
-      </c>
-      <c r="AF9" s="19" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="19" x14ac:dyDescent="0.25">
@@ -3590,21 +4050,21 @@
         <v>10334358000</v>
       </c>
       <c r="AC12" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD12" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="AD12" s="19" t="s">
+      <c r="AE12" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="AE12" s="19" t="s">
+      <c r="AF12" s="19" t="s">
         <v>120</v>
-      </c>
-      <c r="AF12" s="19" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:32" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="15">
         <f>B12/B3</f>
@@ -3853,16 +4313,16 @@
         <v>10334358000</v>
       </c>
       <c r="AC15" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD15" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="AD15" s="19" t="s">
+      <c r="AE15" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="AE15" s="19" t="s">
+      <c r="AF15" s="19" t="s">
         <v>124</v>
-      </c>
-      <c r="AF15" s="19" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:32" ht="19" x14ac:dyDescent="0.25">
@@ -3941,15 +4401,15 @@
       </c>
       <c r="AD16" s="30">
         <f>AE101/W3</f>
-        <v>2.6091664683934659</v>
+        <v>3.0745780799052769</v>
       </c>
       <c r="AE16" s="30">
         <f>AE101/W28</f>
-        <v>23.368597638068803</v>
+        <v>27.536985058822896</v>
       </c>
       <c r="AF16" s="31">
         <f>AE101/W106</f>
-        <v>18.214599244871238</v>
+        <v>21.463639154853304</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -4094,7 +4554,7 @@
         <v>871841000</v>
       </c>
       <c r="AC18" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -4174,7 +4634,7 @@
     </row>
     <row r="20" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="15">
@@ -4832,7 +5292,7 @@
     </row>
     <row r="29" spans="1:29" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="15">
@@ -5277,7 +5737,7 @@
     </row>
     <row r="35" spans="1:23" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="22">
@@ -8491,7 +8951,7 @@
     </row>
     <row r="80" spans="1:23" ht="19" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B80" s="15" t="e">
         <f t="shared" ref="B80:W80" si="6">B79/B3</f>
@@ -8794,10 +9254,10 @@
       <c r="W83" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AD83" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE83" s="34"/>
+      <c r="AD83" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE83" s="57"/>
     </row>
     <row r="84" spans="1:31" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
@@ -8869,10 +9329,10 @@
       <c r="W84" s="1">
         <v>374349000</v>
       </c>
-      <c r="AD84" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE84" s="36"/>
+      <c r="AD84" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE84" s="59"/>
     </row>
     <row r="85" spans="1:31" ht="20" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -8945,7 +9405,7 @@
         <v>648506000</v>
       </c>
       <c r="AD85" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AE85" s="24">
         <f>W17</f>
@@ -9023,7 +9483,7 @@
         <v>1020400000</v>
       </c>
       <c r="AD86" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AE86" s="24">
         <f>W56</f>
@@ -9101,7 +9561,7 @@
         <v>9541129000</v>
       </c>
       <c r="AD87" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AE87" s="24">
         <f>W61</f>
@@ -9178,17 +9638,17 @@
       <c r="W88" s="1">
         <v>-717998000</v>
       </c>
-      <c r="AD88" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE88" s="38">
+      <c r="AD88" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE88" s="34">
         <f>AE85/(AE86+AE87)</f>
         <v>1.4228343871288213E-2</v>
       </c>
     </row>
     <row r="89" spans="1:31" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B89" s="15">
         <f t="shared" ref="B89:W89" si="7">(-1*B88)/B3</f>
@@ -9279,7 +9739,7 @@
         <v>1.1656889382873953E-2</v>
       </c>
       <c r="AD89" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AE89" s="24">
         <f>W27</f>
@@ -9434,10 +9894,10 @@
       <c r="W91" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AD91" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="AE91" s="38">
+      <c r="AD91" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE91" s="34">
         <f>AE89/AE90</f>
         <v>0.24001380140225814</v>
       </c>
@@ -9512,10 +9972,10 @@
       <c r="W92" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AD92" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="AE92" s="40">
+      <c r="AD92" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE92" s="36">
         <f>AE88*(1-AE91)</f>
         <v>1.0813344971081806E-2</v>
       </c>
@@ -9590,10 +10050,10 @@
       <c r="W93" s="1">
         <v>12580000</v>
       </c>
-      <c r="AD93" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="AE93" s="36"/>
+      <c r="AD93" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="AE93" s="59"/>
     </row>
     <row r="94" spans="1:31" ht="20" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
@@ -9666,9 +10126,9 @@
         <v>-4260629000</v>
       </c>
       <c r="AD94" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="AE94" s="41">
+        <v>135</v>
+      </c>
+      <c r="AE94" s="37">
         <v>4.095E-2</v>
       </c>
     </row>
@@ -9742,11 +10202,12 @@
       <c r="W95" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AD95" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="AE95" s="43">
-        <v>1.24</v>
+      <c r="AD95" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE95" s="62" cm="1">
+        <f t="array" ref="AE95">_FV(A1,"Beta")</f>
+        <v>1.2434000000000001</v>
       </c>
     </row>
     <row r="96" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -9820,9 +10281,9 @@
         <v>1349064000</v>
       </c>
       <c r="AD96" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="AE96" s="41">
+        <v>137</v>
+      </c>
+      <c r="AE96" s="37">
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
@@ -9896,12 +10357,12 @@
       <c r="W97" s="1">
         <v>-4116378000</v>
       </c>
-      <c r="AD97" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="AE97" s="40">
+      <c r="AD97" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE97" s="36">
         <f>(AE94)+((AE95)*(AE96-AE94))</f>
-        <v>9.4331999999999999E-2</v>
+        <v>9.4478370000000006E-2</v>
       </c>
     </row>
     <row r="98" spans="1:31" ht="19" x14ac:dyDescent="0.25">
@@ -9974,10 +10435,10 @@
       <c r="W98" s="1">
         <v>-2457306000</v>
       </c>
-      <c r="AD98" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="AE98" s="36"/>
+      <c r="AD98" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE98" s="59"/>
     </row>
     <row r="99" spans="1:31" ht="20" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
@@ -10050,7 +10511,7 @@
         <v>-86406000</v>
       </c>
       <c r="AD99" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE99" s="24">
         <f>AE86+AE87</f>
@@ -10127,12 +10588,12 @@
       <c r="W100" s="10">
         <v>-5311026000</v>
       </c>
-      <c r="AD100" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="AE100" s="38">
+      <c r="AD100" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE100" s="34">
         <f>AE99/AE103</f>
-        <v>2.0274604953967258E-2</v>
+        <v>1.7258521353273621E-2</v>
       </c>
     </row>
     <row r="101" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -10206,11 +10667,11 @@
         <v>-247815000</v>
       </c>
       <c r="AD101" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE101" s="58">
-        <f>W34*Y116</f>
-        <v>160709795250</v>
+        <v>142</v>
+      </c>
+      <c r="AE101" s="49" cm="1">
+        <f t="array" ref="AE101">_FV(A1,"Market cap",TRUE)</f>
+        <v>189376500000</v>
       </c>
     </row>
     <row r="102" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -10283,12 +10744,12 @@
       <c r="W102" s="10">
         <v>-278341000</v>
       </c>
-      <c r="AD102" s="37" t="s">
-        <v>144</v>
-      </c>
-      <c r="AE102" s="38">
+      <c r="AD102" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE102" s="34">
         <f>AE101/AE103</f>
-        <v>0.97972539504603273</v>
+        <v>0.98274147864672634</v>
       </c>
     </row>
     <row r="103" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -10361,12 +10822,12 @@
       <c r="W103" s="1">
         <v>8168174000</v>
       </c>
-      <c r="AD103" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="AE103" s="44">
+      <c r="AD103" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE103" s="38">
         <f>AE99+AE101</f>
-        <v>164035551250</v>
+        <v>192702256000</v>
       </c>
     </row>
     <row r="104" spans="1:31" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -10439,14 +10900,14 @@
       <c r="W104" s="11">
         <v>7889833000</v>
       </c>
-      <c r="AD104" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="AE104" s="36"/>
+      <c r="AD104" s="58" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE104" s="59"/>
     </row>
     <row r="105" spans="1:31" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="15">
@@ -10540,11 +11001,11 @@
       <c r="AB105" s="15"/>
       <c r="AC105" s="15"/>
       <c r="AD105" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AE105" s="26">
         <f>(AE100*AE92)+(AE102*AE97)</f>
-        <v>9.2638692263002004E-2</v>
+        <v>9.3034435379016234E-2</v>
       </c>
     </row>
     <row r="106" spans="1:31" ht="19" x14ac:dyDescent="0.25">
@@ -10617,33 +11078,33 @@
       <c r="W106" s="1">
         <v>8823131000</v>
       </c>
-      <c r="X106" s="45">
+      <c r="X106" s="63">
         <f>W106*(1+$AE$106)</f>
         <v>9348164161.4508705</v>
       </c>
-      <c r="Y106" s="45">
+      <c r="Y106" s="63">
         <f t="shared" ref="Y106:AB106" si="9">X106*(1+$AE$106)</f>
         <v>9904440179.9581642</v>
       </c>
-      <c r="Z106" s="45">
+      <c r="Z106" s="63">
         <f t="shared" si="9"/>
         <v>10493818206.883579</v>
       </c>
-      <c r="AA106" s="45">
+      <c r="AA106" s="63">
         <f t="shared" si="9"/>
         <v>11118268025.077459</v>
       </c>
-      <c r="AB106" s="45">
+      <c r="AB106" s="63">
         <f t="shared" si="9"/>
         <v>11779876632.165413</v>
       </c>
-      <c r="AC106" s="46" t="s">
+      <c r="AC106" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD106" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="AD106" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="AE106" s="48">
+      <c r="AE106" s="41">
         <f>(SUM(X4:AB4)/5)</f>
         <v>5.950644521212136E-2</v>
       </c>
@@ -10672,150 +11133,151 @@
       <c r="U107" s="13"/>
       <c r="V107" s="13"/>
       <c r="W107" s="13"/>
-      <c r="X107" s="46"/>
-      <c r="Y107" s="46"/>
-      <c r="Z107" s="46"/>
-      <c r="AA107" s="46"/>
-      <c r="AB107" s="49">
+      <c r="X107" s="39"/>
+      <c r="Y107" s="39"/>
+      <c r="Z107" s="39"/>
+      <c r="AA107" s="39"/>
+      <c r="AB107" s="42">
         <f>AB106*(1+AE107)/(AE108-AE107)</f>
-        <v>178512817796.95441</v>
-      </c>
-      <c r="AC107" s="50" t="s">
+        <v>177474443356.57159</v>
+      </c>
+      <c r="AC107" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD107" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="AD107" s="51" t="s">
-        <v>150</v>
-      </c>
-      <c r="AE107" s="52">
+      <c r="AE107" s="45">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="108" spans="1:31" ht="19" x14ac:dyDescent="0.25">
-      <c r="X108" s="49">
+      <c r="X108" s="42">
         <f t="shared" ref="X108:Z108" si="10">X107+X106</f>
         <v>9348164161.4508705</v>
       </c>
-      <c r="Y108" s="49">
+      <c r="Y108" s="42">
         <f t="shared" si="10"/>
         <v>9904440179.9581642</v>
       </c>
-      <c r="Z108" s="49">
+      <c r="Z108" s="42">
         <f t="shared" si="10"/>
         <v>10493818206.883579</v>
       </c>
-      <c r="AA108" s="49">
+      <c r="AA108" s="42">
         <f>AA107+AA106</f>
         <v>11118268025.077459</v>
       </c>
-      <c r="AB108" s="49">
+      <c r="AB108" s="42">
         <f>AB107+AB106</f>
-        <v>190292694429.11981</v>
-      </c>
-      <c r="AC108" s="50" t="s">
-        <v>145</v>
-      </c>
-      <c r="AD108" s="53" t="s">
+        <v>189254319988.737</v>
+      </c>
+      <c r="AC108" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD108" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="AE108" s="47">
+        <f>AE105</f>
+        <v>9.3034435379016234E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:31" ht="19" x14ac:dyDescent="0.25">
+      <c r="X109" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="AE108" s="54">
-        <f>AE105</f>
-        <v>9.2638692263002004E-2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:31" ht="19" x14ac:dyDescent="0.25">
-      <c r="X109" s="55" t="s">
+      <c r="Y109" s="61"/>
+    </row>
+    <row r="110" spans="1:31" ht="20" x14ac:dyDescent="0.25">
+      <c r="X110" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="Y109" s="56"/>
-    </row>
-    <row r="110" spans="1:31" ht="20" x14ac:dyDescent="0.25">
-      <c r="X110" s="57" t="s">
+      <c r="Y110" s="49">
+        <f>NPV(AE108,X108,Y108,Z108,AA108,AB108)</f>
+        <v>153972255832.41473</v>
+      </c>
+    </row>
+    <row r="111" spans="1:31" ht="20" x14ac:dyDescent="0.25">
+      <c r="X111" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="Y110" s="58">
-        <f>NPV(AE108,X108,Y108,Z108,AA108,AB108)</f>
-        <v>154887983500.56265</v>
-      </c>
-    </row>
-    <row r="111" spans="1:31" ht="20" x14ac:dyDescent="0.25">
-      <c r="X111" s="57" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y111" s="58">
+      <c r="Y111" s="49">
         <f>W40</f>
         <v>7893806000</v>
       </c>
     </row>
     <row r="112" spans="1:31" ht="20" x14ac:dyDescent="0.25">
-      <c r="X112" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y112" s="58">
+      <c r="X112" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y112" s="49">
         <f>AE99</f>
         <v>3325756000</v>
       </c>
     </row>
     <row r="113" spans="24:25" ht="20" x14ac:dyDescent="0.25">
-      <c r="X113" s="57" t="s">
+      <c r="X113" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y113" s="49">
+        <f>Y110+Y111-Y112</f>
+        <v>158540305832.41473</v>
+      </c>
+    </row>
+    <row r="114" spans="24:25" ht="20" x14ac:dyDescent="0.25">
+      <c r="X114" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="Y113" s="58">
-        <f>Y110+Y111-Y112</f>
-        <v>159456033500.56265</v>
-      </c>
-    </row>
-    <row r="114" spans="24:25" ht="20" x14ac:dyDescent="0.25">
-      <c r="X114" s="57" t="s">
-        <v>156</v>
-      </c>
-      <c r="Y114" s="59">
+      <c r="Y114" s="50">
         <f>W34*(1+(5*AC16))</f>
         <v>625506115.32664871</v>
       </c>
     </row>
     <row r="115" spans="24:25" ht="20" x14ac:dyDescent="0.25">
-      <c r="X115" s="60" t="s">
+      <c r="X115" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y115" s="52">
+        <f>Y113/Y114</f>
+        <v>253.45924196060434</v>
+      </c>
+    </row>
+    <row r="116" spans="24:25" ht="20" x14ac:dyDescent="0.25">
+      <c r="X116" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="Y115" s="61">
-        <f>Y113/Y114</f>
-        <v>254.92322072229831</v>
-      </c>
-    </row>
-    <row r="116" spans="24:25" ht="20" x14ac:dyDescent="0.25">
-      <c r="X116" s="62" t="s">
+      <c r="Y116" s="64" cm="1">
+        <f t="array" ref="Y116">_FV(A1,"Price (Extended hours)",TRUE)</f>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="117" spans="24:25" ht="20" x14ac:dyDescent="0.25">
+      <c r="X117" s="53" t="s">
         <v>158</v>
       </c>
-      <c r="Y116" s="63">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="117" spans="24:25" ht="20" x14ac:dyDescent="0.25">
-      <c r="X117" s="64" t="s">
+      <c r="Y117" s="54">
+        <f>Y115/Y116-1</f>
+        <v>-0.11377887426362121</v>
+      </c>
+    </row>
+    <row r="118" spans="24:25" ht="20" x14ac:dyDescent="0.25">
+      <c r="X118" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="Y117" s="65">
-        <f>Y115/Y116-1</f>
-        <v>1.9692882889193353E-2</v>
-      </c>
-    </row>
-    <row r="118" spans="24:25" ht="20" x14ac:dyDescent="0.25">
-      <c r="X118" s="64" t="s">
-        <v>160</v>
-      </c>
-      <c r="Y118" s="66" t="str">
+      <c r="Y118" s="55" t="str">
         <f>IF(Y115&gt;Y116,"BUY","SELL")</f>
-        <v>BUY</v>
+        <v>SELL</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="X109:Y109"/>
     <mergeCell ref="AD83:AE83"/>
     <mergeCell ref="AD84:AE84"/>
     <mergeCell ref="AD93:AE93"/>
     <mergeCell ref="AD98:AE98"/>
     <mergeCell ref="AD104:AE104"/>
-    <mergeCell ref="X109:Y109"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" tooltip="https://roic.ai/company/ACN" display="ROIC.AI | ACN" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Added alot of models + updated dashboard
</commit_message>
<xml_diff>
--- a/Big Tech/Accenture.xlsx
+++ b/Big Tech/Accenture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Big Tech/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00BEA6D-5F21-D94B-B474-7E39CF484C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A8C365-FF8C-0C4B-86DF-E6D2D9ED6851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -556,11 +556,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,###,,;\(#,###,,\);\ \-\ \-"/>
     <numFmt numFmtId="165" formatCode="#.00%;\ \-#.00%;\ \-\ \-"/>
     <numFmt numFmtId="166" formatCode="#,##0.00_);\(#,##0.00\);\-\ \-"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -997,13 +998,21 @@
     <xf numFmtId="164" fontId="1" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="11" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1017,15 +1026,7 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="39" fontId="11" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="12" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2375,13 +2376,13 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>345.29500000000002</v>
+    <v>344.81</v>
     <v>242.8</v>
-    <v>1.2434000000000001</v>
-    <v>3.15</v>
-    <v>1.1144000000000001E-2</v>
-    <v>0.19</v>
-    <v>6.648E-4</v>
+    <v>1.2435</v>
+    <v>0.37</v>
+    <v>1.315E-3</v>
+    <v>-0.19</v>
+    <v>-6.7449999999999997E-4</v>
     <v>USD</v>
     <v>Accenture plc is a global professional services company engaged in providing a range of services in strategy and consulting, technology, operations and Accenture song. It serves clients in North America, Europe and Growth markets. It provides a range of services, including application services, artificial intelligence, automation, business process outsourcing, business strategy, change management, cloud, data and analytics, digital commerce, digital engineering and manufacturing, finance consulting, infrastructure, marketing, mergers and acquisitions, metaverse, operating models, security, supply chain management, technology consulting, technology innovation and zero-based transformation. It helps organizations to achieve transformational impact with solutions in C-Suite assessment, team dynamics and various others. It also offers automated production lines that leverage the cloud, data and artificial intelligence (AI) that makes factories and plants smarter through Eclipse Automation.</v>
     <v>721000</v>
@@ -2389,25 +2390,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>1 Grand Canal Square, Grand Canal Harbour, Dublin 2, DUBLIN, DUBLIN IE</v>
-    <v>285.95999999999998</v>
+    <v>282.24</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45016.992773471873</v>
+    <v>45022.996718622657</v>
     <v>0</v>
-    <v>282.61</v>
-    <v>189376500000</v>
+    <v>278.86</v>
+    <v>186653200000</v>
     <v>ACCENTURE PUBLIC LIMITED COMPANY</v>
     <v>ACCENTURE PUBLIC LIMITED COMPANY</v>
-    <v>283.12</v>
-    <v>26.017099999999999</v>
-    <v>282.66000000000003</v>
-    <v>285.81</v>
-    <v>286</v>
+    <v>280.66000000000003</v>
+    <v>25.8947</v>
+    <v>281.33</v>
+    <v>281.7</v>
+    <v>281.51</v>
     <v>662595700</v>
     <v>ACN</v>
     <v>ACCENTURE PUBLIC LIMITED COMPANY (XNYS:ACN)</v>
-    <v>3009370</v>
-    <v>2885890</v>
+    <v>2125329</v>
+    <v>3009610</v>
     <v>2009</v>
   </rv>
   <rv s="2">
@@ -2995,10 +2996,10 @@
   <dimension ref="A1:AF118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Y124" sqref="Y124"/>
+      <selection pane="bottomRight" activeCell="Y115" sqref="Y115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4401,15 +4402,15 @@
       </c>
       <c r="AD16" s="30">
         <f>AE101/W3</f>
-        <v>3.0745780799052769</v>
+        <v>3.0303645767250722</v>
       </c>
       <c r="AE16" s="30">
         <f>AE101/W28</f>
-        <v>27.536985058822896</v>
+        <v>27.140993626883386</v>
       </c>
       <c r="AF16" s="31">
         <f>AE101/W106</f>
-        <v>21.463639154853304</v>
+        <v>21.154984551402443</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -9254,10 +9255,10 @@
       <c r="W83" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AD83" s="56" t="s">
+      <c r="AD83" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="AE83" s="57"/>
+      <c r="AE83" s="61"/>
     </row>
     <row r="84" spans="1:31" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
@@ -9329,10 +9330,10 @@
       <c r="W84" s="1">
         <v>374349000</v>
       </c>
-      <c r="AD84" s="58" t="s">
+      <c r="AD84" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="AE84" s="59"/>
+      <c r="AE84" s="63"/>
     </row>
     <row r="85" spans="1:31" ht="20" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -10050,10 +10051,10 @@
       <c r="W93" s="1">
         <v>12580000</v>
       </c>
-      <c r="AD93" s="58" t="s">
+      <c r="AD93" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="AE93" s="59"/>
+      <c r="AE93" s="63"/>
     </row>
     <row r="94" spans="1:31" ht="20" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
@@ -10205,9 +10206,9 @@
       <c r="AD95" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="AE95" s="62" cm="1">
+      <c r="AE95" s="55" cm="1">
         <f t="array" ref="AE95">_FV(A1,"Beta")</f>
-        <v>1.2434000000000001</v>
+        <v>1.2435</v>
       </c>
     </row>
     <row r="96" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -10362,7 +10363,7 @@
       </c>
       <c r="AE97" s="36">
         <f>(AE94)+((AE95)*(AE96-AE94))</f>
-        <v>9.4478370000000006E-2</v>
+        <v>9.4482675000000016E-2</v>
       </c>
     </row>
     <row r="98" spans="1:31" ht="19" x14ac:dyDescent="0.25">
@@ -10435,10 +10436,10 @@
       <c r="W98" s="1">
         <v>-2457306000</v>
       </c>
-      <c r="AD98" s="58" t="s">
+      <c r="AD98" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="AE98" s="59"/>
+      <c r="AE98" s="63"/>
     </row>
     <row r="99" spans="1:31" ht="20" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
@@ -10593,7 +10594,7 @@
       </c>
       <c r="AE100" s="34">
         <f>AE99/AE103</f>
-        <v>1.7258521353273621E-2</v>
+        <v>1.7505917865976692E-2</v>
       </c>
     </row>
     <row r="101" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -10671,7 +10672,7 @@
       </c>
       <c r="AE101" s="49" cm="1">
         <f t="array" ref="AE101">_FV(A1,"Market cap",TRUE)</f>
-        <v>189376500000</v>
+        <v>186653200000</v>
       </c>
     </row>
     <row r="102" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -10749,7 +10750,7 @@
       </c>
       <c r="AE102" s="34">
         <f>AE101/AE103</f>
-        <v>0.98274147864672634</v>
+        <v>0.98249408213402334</v>
       </c>
     </row>
     <row r="103" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -10827,7 +10828,7 @@
       </c>
       <c r="AE103" s="38">
         <f>AE99+AE101</f>
-        <v>192702256000</v>
+        <v>189978956000</v>
       </c>
     </row>
     <row r="104" spans="1:31" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -10900,10 +10901,10 @@
       <c r="W104" s="11">
         <v>7889833000</v>
       </c>
-      <c r="AD104" s="58" t="s">
+      <c r="AD104" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="AE104" s="59"/>
+      <c r="AE104" s="63"/>
     </row>
     <row r="105" spans="1:31" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
@@ -11005,7 +11006,7 @@
       </c>
       <c r="AE105" s="26">
         <f>(AE100*AE92)+(AE102*AE97)</f>
-        <v>9.3034435379016234E-2</v>
+        <v>9.3017966580612482E-2</v>
       </c>
     </row>
     <row r="106" spans="1:31" ht="19" x14ac:dyDescent="0.25">
@@ -11078,23 +11079,23 @@
       <c r="W106" s="1">
         <v>8823131000</v>
       </c>
-      <c r="X106" s="63">
+      <c r="X106" s="56">
         <f>W106*(1+$AE$106)</f>
         <v>9348164161.4508705</v>
       </c>
-      <c r="Y106" s="63">
+      <c r="Y106" s="56">
         <f t="shared" ref="Y106:AB106" si="9">X106*(1+$AE$106)</f>
         <v>9904440179.9581642</v>
       </c>
-      <c r="Z106" s="63">
+      <c r="Z106" s="56">
         <f t="shared" si="9"/>
         <v>10493818206.883579</v>
       </c>
-      <c r="AA106" s="63">
+      <c r="AA106" s="56">
         <f t="shared" si="9"/>
         <v>11118268025.077459</v>
       </c>
-      <c r="AB106" s="63">
+      <c r="AB106" s="56">
         <f t="shared" si="9"/>
         <v>11779876632.165413</v>
       </c>
@@ -11139,7 +11140,7 @@
       <c r="AA107" s="39"/>
       <c r="AB107" s="42">
         <f>AB106*(1+AE107)/(AE108-AE107)</f>
-        <v>177474443356.57159</v>
+        <v>177517414221.12976</v>
       </c>
       <c r="AC107" s="43" t="s">
         <v>148</v>
@@ -11170,7 +11171,7 @@
       </c>
       <c r="AB108" s="42">
         <f>AB107+AB106</f>
-        <v>189254319988.737</v>
+        <v>189297290853.29517</v>
       </c>
       <c r="AC108" s="43" t="s">
         <v>144</v>
@@ -11180,14 +11181,14 @@
       </c>
       <c r="AE108" s="47">
         <f>AE105</f>
-        <v>9.3034435379016234E-2</v>
+        <v>9.3017966580612482E-2</v>
       </c>
     </row>
     <row r="109" spans="1:31" ht="19" x14ac:dyDescent="0.25">
-      <c r="X109" s="60" t="s">
+      <c r="X109" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="Y109" s="61"/>
+      <c r="Y109" s="59"/>
     </row>
     <row r="110" spans="1:31" ht="20" x14ac:dyDescent="0.25">
       <c r="X110" s="48" t="s">
@@ -11195,7 +11196,7 @@
       </c>
       <c r="Y110" s="49">
         <f>NPV(AE108,X108,Y108,Z108,AA108,AB108)</f>
-        <v>153972255832.41473</v>
+        <v>154010150804.03229</v>
       </c>
     </row>
     <row r="111" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -11222,7 +11223,7 @@
       </c>
       <c r="Y113" s="49">
         <f>Y110+Y111-Y112</f>
-        <v>158540305832.41473</v>
+        <v>158578200804.03229</v>
       </c>
     </row>
     <row r="114" spans="24:25" ht="20" x14ac:dyDescent="0.25">
@@ -11238,34 +11239,34 @@
       <c r="X115" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="Y115" s="52">
+      <c r="Y115" s="64">
         <f>Y113/Y114</f>
-        <v>253.45924196060434</v>
+        <v>253.51982485610131</v>
       </c>
     </row>
     <row r="116" spans="24:25" ht="20" x14ac:dyDescent="0.25">
       <c r="X116" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="Y116" s="64" cm="1">
+      <c r="Y116" s="57" cm="1">
         <f t="array" ref="Y116">_FV(A1,"Price (Extended hours)",TRUE)</f>
-        <v>286</v>
+        <v>281.51</v>
       </c>
     </row>
     <row r="117" spans="24:25" ht="20" x14ac:dyDescent="0.25">
-      <c r="X117" s="53" t="s">
+      <c r="X117" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="Y117" s="54">
+      <c r="Y117" s="53">
         <f>Y115/Y116-1</f>
-        <v>-0.11377887426362121</v>
+        <v>-9.9428706418595025E-2</v>
       </c>
     </row>
     <row r="118" spans="24:25" ht="20" x14ac:dyDescent="0.25">
-      <c r="X118" s="53" t="s">
+      <c r="X118" s="52" t="s">
         <v>159</v>
       </c>
-      <c r="Y118" s="55" t="str">
+      <c r="Y118" s="54" t="str">
         <f>IF(Y115&gt;Y116,"BUY","SELL")</f>
         <v>SELL</v>
       </c>

</xml_diff>